<commit_message>
umm....lots of updates. Both SSO orbits and now iridium stuff
</commit_message>
<xml_diff>
--- a/SSO/parameters_descope_2.xlsx
+++ b/SSO/parameters_descope_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19220" tabRatio="500" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19080" tabRatio="500" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="sim_parameters" sheetId="5" r:id="rId1"/>
@@ -314,8 +314,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -334,17 +336,19 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="40" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -790,7 +794,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75">
+    <row r="1" spans="1:8" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -816,7 +820,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75">
+    <row r="2" spans="1:8" ht="18">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -842,7 +846,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75">
+    <row r="3" spans="1:8" ht="18">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -868,7 +872,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75">
+    <row r="4" spans="1:8" ht="18">
       <c r="H4" s="1" t="s">
         <v>20</v>
       </c>
@@ -897,7 +901,7 @@
     <col min="7" max="7" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75">
+    <row r="1" spans="1:8" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -923,7 +927,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75">
+    <row r="2" spans="1:8" ht="18">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -950,7 +954,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75">
+    <row r="3" spans="1:8" ht="18">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -977,7 +981,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75">
+    <row r="4" spans="1:8" ht="18">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1004,7 +1008,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75">
+    <row r="5" spans="1:8" ht="18">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1047,13 +1051,14 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1140,6 +1145,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1153,7 +1159,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>